<commit_message>
wip: new assignment method
</commit_message>
<xml_diff>
--- a/input/24/pre-assigned.xlsx
+++ b/input/24/pre-assigned.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,18 +436,21 @@
         <v>Salle</v>
       </c>
       <c r="K1" t="str">
-        <v>Marqueur 1</v>
+        <v>Responsable du match</v>
       </c>
       <c r="L1" t="str">
-        <v>Marqueur 2</v>
+        <v>Marqueur principal</v>
       </c>
       <c r="M1" t="str">
-        <v>Téléphone marqueur 1</v>
+        <v>Tél. marqueur principal</v>
       </c>
       <c r="N1" t="str">
-        <v>Téléphone marqueur 2</v>
+        <v>Marqueur assistant</v>
       </c>
       <c r="O1" t="str">
+        <v>Tél. marqueur assistant</v>
+      </c>
+      <c r="P1" t="str">
         <v>Commentaire</v>
       </c>
     </row>
@@ -494,6 +497,9 @@
       <c r="N2" t="str">
         <v/>
       </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -878,7 +884,7 @@
       <c r="J14" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P14" t="str">
         <v>2 matchs en 2 sets - 362298 / 362277</v>
       </c>
     </row>
@@ -2385,7 +2391,7 @@
       <c r="J61" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
-      <c r="O61" t="str">
+      <c r="P61" t="str">
         <v>2 matchs en 2 sets - 362272 / 362293</v>
       </c>
     </row>
@@ -2775,7 +2781,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O73"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P73"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>